<commit_message>
Add 'Historique' link to sushi-config.yaml ebbb6a9b9d9ad7d40ea0cf49972b860fdc9c33c0
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-fr-patient.xlsx
+++ b/main/ig/StructureDefinition-fr-patient.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-08-21T09:52:50+00:00</t>
+    <t>2025-11-14T15:31:38+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -371,7 +371,7 @@
     <t>A human language.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/languages</t>
+    <t>http://hl7.org/fhir/ValueSet/languages|4.0.1</t>
   </si>
   <si>
     <t>Resource.language</t>
@@ -641,7 +641,7 @@
     <t>A coded type for an identifier that can be used to determine which identifier to use for a specific purpose.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/identifier-type</t>
+    <t>http://hl7.org/fhir/ValueSet/identifier-type|4.0.1</t>
   </si>
   <si>
     <t>Identifier.type</t>
@@ -741,7 +741,7 @@
     <t>Patient.identifier.assigner</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Organization)
+    <t xml:space="preserve">Reference(Organization|4.0.1)
 </t>
   </si>
   <si>
@@ -976,7 +976,7 @@
     <t>The domestic partnership status of a person.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/marital-status</t>
+    <t>http://hl7.org/fhir/ValueSet/marital-status|4.0.1</t>
   </si>
   <si>
     <t>player[classCode=PSN]/maritalStatusCode</t>
@@ -1105,7 +1105,7 @@
     <t>The nature of the relationship between a patient and a contact person for that patient.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/patient-contactrelationship</t>
+    <t>http://hl7.org/fhir/ValueSet/patient-contactrelationship|4.0.1</t>
   </si>
   <si>
     <t>code</t>
@@ -1299,7 +1299,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Organization|Practitioner|PractitionerRole)
+    <t xml:space="preserve">Reference(Organization|4.0.1|Practitioner|4.0.1|PractitionerRole|4.0.1)
 </t>
   </si>
   <si>
@@ -1370,7 +1370,7 @@
     <t>Patient.link.other</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Patient|RelatedPerson)
+    <t xml:space="preserve">Reference(Patient|4.0.1|RelatedPerson|4.0.1)
 </t>
   </si>
   <si>
@@ -2822,7 +2822,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" hidden="true">
+    <row r="10">
       <c r="A10" t="s" s="2">
         <v>141</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" hidden="true">
+    <row r="13">
       <c r="A13" t="s" s="2">
         <v>165</v>
       </c>
@@ -8357,12 +8357,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AO56">
-    <filterColumn colId="6">
+    <filterColumn colId="7">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
-    <filterColumn colId="26">
+    <filterColumn colId="27">
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>

</xml_diff>